<commit_message>
Cambios consultas base de datos, y revision contabilidad alumnos
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>MODULO</t>
   </si>
@@ -170,9 +170,6 @@
     <t>SE PRUEBA LA IMPRESIÓN DIRECTA DE CARNETS LA CUAL SALE SATISFACTORIA</t>
   </si>
   <si>
-    <t>SE AJUSTAS XML A POSICIONES SEGÚN IMAGEN ENVIADA, SE QUEDA A LA ESPERA DE CONFIRMACION SI ES LA POSICION CORRECTA PARA LOS DATOS</t>
-  </si>
-  <si>
     <t>SE AJUSTA EL PASO DE ALUMNOS PARA LOS DIAS AUTORIZADOS</t>
   </si>
   <si>
@@ -182,22 +179,31 @@
     <t>SE AGREGA ADVERTENCIA CUANDO EL USUARIO TIENE RESTRICCIONES MEDICAS</t>
   </si>
   <si>
-    <t>ARREGLO FALLO QUE PERMITE EL PASO DE UN USUARIO OVARIAS VECES EL MISMO DIAS, CUANDO EL USUARIO PASA DE NUEVO MUESTRA ALERTA</t>
-  </si>
-  <si>
     <t>SE AJUSTO EL INCONVENIENTE POR FAVOR PROBAR DE NUEVO</t>
   </si>
   <si>
     <t>SE AJUSTA EL FORMATO DE IMPRESIÓN PARA TODAS LAS ORLAS PENDIENTE VERIFICACION</t>
   </si>
   <si>
-    <t>SE AJUSTA EL CORTE DE LA IMAGEN AL TAMAÑO SOLICITADO</t>
-  </si>
-  <si>
     <t>SE AJUSTA BUSQUEDA DE IMÁGENES</t>
   </si>
   <si>
     <t>EVIDENCIA DE MANTENIMIENTO</t>
+  </si>
+  <si>
+    <t>INCONVENIENTES DESPUES DEL CAMBIO</t>
+  </si>
+  <si>
+    <t>SE GENERA LOS CARNETS PERO SALE CON ERRORES AL GENERAR ALGUNOS PDFS</t>
+  </si>
+  <si>
+    <t>SE AJUSTAS XML A POSICIONES SEGÚN IMAGEN ENVIADA, SE QUEDA A LA ESPERA DE CONFIRMACION SI ES LA POSICION CORRECTA PARA LOS DATOS, TAMBIEN SE REALIZA AJUSTE DE LA POSICION DEL CODIGO DE BARRAS</t>
+  </si>
+  <si>
+    <t>ARREGLO FALLO QUE PERMITE EL PASO DE UN USUARIO OVARIAS VECES EL MISMO DIAS, CUANDO EL USUARIO PASA DE NUEVO NO CONTABILIZA EL PASO DEL USUARIO</t>
+  </si>
+  <si>
+    <t>SE AJUSTA PARA QUE AL MOMENTO DE REALIZAR EL CORTE DE LA IMAGEN LA AJUSTE AL FORMATO 480 X 640</t>
   </si>
 </sst>
 </file>
@@ -282,9 +288,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,9 +297,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -327,34 +327,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -550,44 +539,6 @@
         <a:xfrm>
           <a:off x="8477249" y="17371218"/>
           <a:ext cx="4085714" cy="1200000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>369094</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>4094260</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2040585</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8560593" y="11513344"/>
-          <a:ext cx="3737073" cy="1671491"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -894,444 +845,449 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="216" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="69.85546875" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="15" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="E5" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="7" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F7" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="15" t="s">
+    <row r="11" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="B24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="216" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="C28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1340,7 +1296,7 @@
     <sortCondition ref="A2:A21" customList="CARNETS,INFORMES Y REPORTES,AUTORIZADOS,REGISTRO Y ACTUALIZACION DE DATOS,CONTROL PRESENCIA,CONTABILIDAD ALUMNOS,CONTABILIDAD PROFESORES"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>